<commit_message>
Tackling part of mod 1 quiz
</commit_message>
<xml_diff>
--- a/Module 1 - Quiz/Module 1_Quiz CAGR.xlsx
+++ b/Module 1 - Quiz/Module 1_Quiz CAGR.xlsx
@@ -1,20 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CertTFS\Online-Content\Courses\ENG\DAT222x - Essential Statistics for Data Analysis using Excel\Assessments\Module 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anguyen\Documents\GitHub\stats-edx\Module 1 - Quiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88547DB6-F7B1-4871-9244-4DD5623E2664}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7890" windowHeight="6458"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7890" windowHeight="6465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAGR" sheetId="7" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -36,10 +44,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="168" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -89,16 +99,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -435,16 +449,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
@@ -458,7 +475,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2007</v>
       </c>
@@ -475,7 +492,7 @@
         <v>-1.8639534282121062E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2008</v>
       </c>
@@ -492,7 +509,7 @@
         <v>3.0986857795568312E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2009</v>
       </c>
@@ -509,7 +526,7 @@
         <v>2.2705310921699029E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2010</v>
       </c>
@@ -526,7 +543,7 @@
         <v>-1.0609956363902162E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2011</v>
       </c>
@@ -543,7 +560,7 @@
         <v>1.4882914589414931E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2012</v>
       </c>
@@ -560,7 +577,7 @@
         <v>5.0802355917638486E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2013</v>
       </c>
@@ -577,7 +594,7 @@
         <v>3.0795425260179199E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2014</v>
       </c>
@@ -594,7 +611,7 @@
         <v>-4.6480689583271118E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2015</v>
       </c>
@@ -611,7 +628,7 @@
         <v>2.4836661377807712E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2016</v>
       </c>
@@ -626,6 +643,244 @@
       </c>
       <c r="E11" s="1">
         <v>7.444330513921571E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <f>A2</f>
+        <v>2007</v>
+      </c>
+      <c r="B13" s="3">
+        <f>B2+1</f>
+        <v>0.90423495402383469</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" ref="C13:E13" si="0">C2+1</f>
+        <v>0.99217176912658134</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="0"/>
+        <v>0.98994336584972054</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>0.99813604657178789</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <f t="shared" ref="A14:A21" si="1">A3</f>
+        <v>2008</v>
+      </c>
+      <c r="B14" s="3">
+        <f t="shared" ref="B14:E14" si="2">B3+1</f>
+        <v>0.94259994391319857</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0017904667089472</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="2"/>
+        <v>0.9890403250631814</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0309868577955683</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <f t="shared" si="1"/>
+        <v>2009</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" ref="B15:E15" si="3">B4+1</f>
+        <v>0.95685779095053658</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="3"/>
+        <v>0.99742484723545766</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="3"/>
+        <v>0.9998518566872826</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="3"/>
+        <v>1.022705310921699</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <f t="shared" si="1"/>
+        <v>2010</v>
+      </c>
+      <c r="B16" s="3">
+        <f t="shared" ref="B16:E16" si="4">B5+1</f>
+        <v>0.97213390135747135</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" si="4"/>
+        <v>0.99732669059794876</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="4"/>
+        <v>1.0048081957911019</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="4"/>
+        <v>0.98939004363609784</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <f t="shared" si="1"/>
+        <v>2011</v>
+      </c>
+      <c r="B17" s="3">
+        <f t="shared" ref="B17:E17" si="5">B6+1</f>
+        <v>0.97950872501348851</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0006466597809565</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0203931094109708</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0148829145894149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <f t="shared" si="1"/>
+        <v>2012</v>
+      </c>
+      <c r="B18" s="3">
+        <f t="shared" ref="B18:E18" si="6">B7+1</f>
+        <v>0.99197395903631114</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="6"/>
+        <v>1.0078167133006277</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="6"/>
+        <v>1.0111716930826093</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="6"/>
+        <v>1.0050802355917638</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <f t="shared" si="1"/>
+        <v>2013</v>
+      </c>
+      <c r="B19" s="3">
+        <f t="shared" ref="B19:E19" si="7">B8+1</f>
+        <v>1.0055654689993045</v>
+      </c>
+      <c r="C19" s="3">
+        <f t="shared" si="7"/>
+        <v>0.99986357493256361</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="7"/>
+        <v>1.0392056932890286</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="7"/>
+        <v>1.0307954252601792</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <f t="shared" si="1"/>
+        <v>2014</v>
+      </c>
+      <c r="B20" s="3">
+        <f t="shared" ref="B20:E20" si="8">B9+1</f>
+        <v>1.0242318367931802</v>
+      </c>
+      <c r="C20" s="3">
+        <f t="shared" si="8"/>
+        <v>1.0147252523961343</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="8"/>
+        <v>0.98077231133751652</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="8"/>
+        <v>0.95351931041672888</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <f t="shared" si="1"/>
+        <v>2015</v>
+      </c>
+      <c r="B21" s="3">
+        <f t="shared" ref="B21:E22" si="9">B10+1</f>
+        <v>1.0499804877471572</v>
+      </c>
+      <c r="C21" s="3">
+        <f t="shared" si="9"/>
+        <v>1.0016818150586844</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="9"/>
+        <v>1.0101145561775675</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="9"/>
+        <v>1.0248366613778077</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <f>A11</f>
+        <v>2016</v>
+      </c>
+      <c r="B22" s="3">
+        <f>B11+1</f>
+        <v>1.1158681577307215</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" si="9"/>
+        <v>1.0569848989927986</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="9"/>
+        <v>1.0093496276192848</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="9"/>
+        <v>1.0074443305139216</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="4">
+        <f>GEOMEAN(B13:B22)-1</f>
+        <v>-7.2741055445060265E-3</v>
+      </c>
+      <c r="C23" s="4">
+        <f t="shared" ref="C23:E23" si="10">GEOMEAN(C13:C22)-1</f>
+        <v>6.8925972297757543E-3</v>
+      </c>
+      <c r="D23" s="4">
+        <f t="shared" si="10"/>
+        <v>5.3372086777021543E-3</v>
+      </c>
+      <c r="E23" s="4">
+        <f t="shared" si="10"/>
+        <v>7.5242955463439287E-3</v>
       </c>
     </row>
   </sheetData>
@@ -634,15 +889,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AF8E4BBD310ADB419B3C5F1ACE4D113D" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="63e1bd94a874076348984a0131457edc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d1607db4-bd3f-4f82-a312-bf7e283d0a6b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7c9989741aedae2f07a76d9f40ef2a18" ns2:_="">
     <xsd:import namespace="d1607db4-bd3f-4f82-a312-bf7e283d0a6b"/>
@@ -702,6 +948,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
@@ -711,14 +966,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DA1585F-B771-4D19-B45A-254B2B3993AE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEAB0E56-AF27-40AE-BC71-146452798C0D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -731,6 +978,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DA1585F-B771-4D19-B45A-254B2B3993AE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>